<commit_message>
update onboarding survey with alternate formats
</commit_message>
<xml_diff>
--- a/survey_resources/dfc-fermata/fermata-onboarding-v0.xlsx
+++ b/survey_resources/dfc-fermata/fermata-onboarding-v0.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="138">
   <si>
     <t>type</t>
   </si>
@@ -156,25 +156,22 @@
     <t>Have you ever driven an EV and/or use an electrical charging station?</t>
   </si>
   <si>
-    <t>Please_rate_the_following_statements</t>
-  </si>
-  <si>
-    <t>field-list</t>
-  </si>
-  <si>
-    <t>select_one kt2eu04</t>
-  </si>
-  <si>
-    <t>Please_rate_the_following_statements_header</t>
-  </si>
-  <si>
-    <t>Please rate the following statements:</t>
-  </si>
-  <si>
-    <t>1 = disagree, 2 = somewhat disagree, 3 = neutral, 4 = somewhat agree, 5 = agree</t>
-  </si>
-  <si>
-    <t>label</t>
+    <t>acknowledge</t>
+  </si>
+  <si>
+    <t>Acknowledge</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>For_each_of_the_foll_e_with_the_statement</t>
+  </si>
+  <si>
+    <t>For each of the following statements, please indicate the extent to which you agree with the statement.</t>
+  </si>
+  <si>
+    <t>select_one ml6mb78</t>
   </si>
   <si>
     <t>The_information_you_l_your_driving_needs</t>
@@ -183,13 +180,19 @@
     <t>The information you have about electric vehicles and charging electric infrastructure is enough to fulfill your driving needs</t>
   </si>
   <si>
-    <t>list-nolabel</t>
+    <t>select_one om8ix13</t>
   </si>
   <si>
     <t>You_are_concerned_th_charging_opportunity</t>
   </si>
   <si>
-    <t>You are concerned that the electric vehicle would run out of charge before the next charging opportunity</t>
+    <t>You are concerned that an electric vehicle could run out of charge before the next charging opportunity</t>
+  </si>
+  <si>
+    <t>horizontal-compact</t>
+  </si>
+  <si>
+    <t>select_one ak2us99</t>
   </si>
   <si>
     <t>Concern_of_running_o_ectric_fleet_vehicle</t>
@@ -198,18 +201,33 @@
     <t>Concern of running out of charge, or range anxiety, prevents you from choosing an electric fleet vehicle</t>
   </si>
   <si>
+    <t>likert</t>
+  </si>
+  <si>
+    <t>select_one vj3vs28</t>
+  </si>
+  <si>
     <t>You_believe_that_the_an_electric_vehicle</t>
   </si>
   <si>
     <t>You believe that the number of electric vehicles charging stations are few within your area of operation and it is a significant obstacle to driving an electric vehicle</t>
   </si>
   <si>
+    <t>compact</t>
+  </si>
+  <si>
+    <t>select_one wq0ck21</t>
+  </si>
+  <si>
     <t>The_use_of_public_ra_nimize_range_anxiety</t>
   </si>
   <si>
     <t>The use of public rapid-charging infrastructure as a back-up option would minimize range anxiety</t>
   </si>
   <si>
+    <t>quickcompact</t>
+  </si>
+  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -363,22 +381,49 @@
     <t>ro8kj99</t>
   </si>
   <si>
-    <t>kt2eu04</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t>ml6mb78</t>
+  </si>
+  <si>
+    <t>disagree</t>
+  </si>
+  <si>
+    <t>Disagree</t>
+  </si>
+  <si>
+    <t>somewhat_disagree</t>
+  </si>
+  <si>
+    <t>Somewhat disagree</t>
+  </si>
+  <si>
+    <t>neither_agree_nor_disagree</t>
+  </si>
+  <si>
+    <t>Neither agree nor disagree</t>
+  </si>
+  <si>
+    <t>somewhat_agree</t>
+  </si>
+  <si>
+    <t>Somewhat agree</t>
+  </si>
+  <si>
+    <t>agree</t>
+  </si>
+  <si>
+    <t>Agree</t>
+  </si>
+  <si>
+    <t>om8ix13</t>
+  </si>
+  <si>
+    <t>ak2us99</t>
+  </si>
+  <si>
+    <t>vj3vs28</t>
+  </si>
+  <si>
+    <t>wq0ck21</t>
   </si>
   <si>
     <t>default_language</t>
@@ -716,7 +761,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -947,30 +992,21 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
-      <c r="G19" t="s">
-        <v>52</v>
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -978,94 +1014,95 @@
         <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
         <v>61</v>
-      </c>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>27</v>
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1075,7 +1112,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1083,7 +1120,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1092,29 +1129,29 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1122,13 +1159,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1136,13 +1173,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1150,13 +1187,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1164,13 +1201,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1178,13 +1215,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1192,277 +1229,497 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B27" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C27" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B28" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B31" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C33" t="s">
-        <v>120</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" t="s">
+        <v>122</v>
+      </c>
+      <c r="C49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>135</v>
+      </c>
+      <c r="B51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1480,12 +1737,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>